<commit_message>
added SCT rank and -1 to adwDF
</commit_message>
<xml_diff>
--- a/data/excel files/in/FlightPersonnel.xlsx
+++ b/data/excel files/in/FlightPersonnel.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="159">
   <si>
     <t>callsign</t>
   </si>
@@ -89,6 +89,9 @@
     <t>NIL</t>
   </si>
   <si>
+    <t>SCT</t>
+  </si>
+  <si>
     <t>CPT</t>
   </si>
   <si>
@@ -119,6 +122,33 @@
     <t>3SG</t>
   </si>
   <si>
+    <t>BRAYDEN</t>
+  </si>
+  <si>
+    <t>NOAH LAM</t>
+  </si>
+  <si>
+    <t>MARCUS</t>
+  </si>
+  <si>
+    <t>MENG LONG</t>
+  </si>
+  <si>
+    <t>KAI</t>
+  </si>
+  <si>
+    <t>CHARLES</t>
+  </si>
+  <si>
+    <t>DARSHAN</t>
+  </si>
+  <si>
+    <t>ZHONG PING</t>
+  </si>
+  <si>
+    <t>DERRILL</t>
+  </si>
+  <si>
     <t>WEI JIAN</t>
   </si>
   <si>
@@ -128,13 +158,13 @@
     <t>JOVAN</t>
   </si>
   <si>
+    <t>RICHMOND</t>
+  </si>
+  <si>
     <t>MAX</t>
   </si>
   <si>
-    <t>RICHMOND RAY</t>
-  </si>
-  <si>
-    <t>LEON LAI</t>
+    <t>LEON</t>
   </si>
   <si>
     <t>YEN KIT</t>
@@ -363,9 +393,6 @@
   </si>
   <si>
     <t>1WO</t>
-  </si>
-  <si>
-    <t>MARCUS</t>
   </si>
   <si>
     <t>KENNETH</t>
@@ -970,7 +997,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1014,7 +1041,7 @@
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1022,16 +1049,16 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1039,16 +1066,16 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1056,475 +1083,628 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" t="s">
-        <v>76</v>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1566,7 +1746,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1578,12 +1758,12 @@
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -1592,15 +1772,15 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -1612,432 +1792,432 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2079,24 +2259,24 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -2105,350 +2285,350 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="D10" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="D11" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="D12" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="D15" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D16" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="C18" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some statuses :)
</commit_message>
<xml_diff>
--- a/data/excel files/in/FlightPersonnel.xlsx
+++ b/data/excel files/in/FlightPersonnel.xlsx
@@ -7,18 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="INSTRUCTIONS" sheetId="1" r:id="rId1"/>
-    <sheet name="CALLSIGN" sheetId="2" r:id="rId2"/>
-    <sheet name="ALPHA" sheetId="3" r:id="rId3"/>
-    <sheet name="BRAVO" sheetId="4" r:id="rId4"/>
-    <sheet name="OTHERS" sheetId="5" r:id="rId5"/>
+    <sheet name="CALLSIGN" sheetId="1" r:id="rId1"/>
+    <sheet name="ALPHA" sheetId="2" r:id="rId2"/>
+    <sheet name="BRAVO" sheetId="3" r:id="rId3"/>
+    <sheet name="OTHERS" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="164">
   <si>
     <t>callsign</t>
   </si>
@@ -89,37 +88,121 @@
     <t>NIL</t>
   </si>
   <si>
+    <t>CPT</t>
+  </si>
+  <si>
+    <t>LTA</t>
+  </si>
+  <si>
+    <t>2LT</t>
+  </si>
+  <si>
+    <t>2WO</t>
+  </si>
+  <si>
+    <t>3WO</t>
+  </si>
+  <si>
+    <t>MSG</t>
+  </si>
+  <si>
+    <t>SSG</t>
+  </si>
+  <si>
+    <t>1SG</t>
+  </si>
+  <si>
+    <t>2SG</t>
+  </si>
+  <si>
+    <t>3SG</t>
+  </si>
+  <si>
     <t>SCT</t>
   </si>
   <si>
-    <t>CPT</t>
-  </si>
-  <si>
-    <t>LTA</t>
-  </si>
-  <si>
-    <t>2LT</t>
-  </si>
-  <si>
-    <t>2WO</t>
-  </si>
-  <si>
-    <t>3WO</t>
-  </si>
-  <si>
-    <t>MSG</t>
-  </si>
-  <si>
-    <t>SSG</t>
-  </si>
-  <si>
-    <t>1SG</t>
-  </si>
-  <si>
-    <t>2SG</t>
-  </si>
-  <si>
-    <t>3SG</t>
+    <t>WEI JIAN</t>
+  </si>
+  <si>
+    <t>BRENDON</t>
+  </si>
+  <si>
+    <t>JOVAN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>RICHMOND</t>
+  </si>
+  <si>
+    <t>LEON</t>
+  </si>
+  <si>
+    <t>YEN KIT</t>
+  </si>
+  <si>
+    <t>AIDAN</t>
+  </si>
+  <si>
+    <t>GUAN LIN</t>
+  </si>
+  <si>
+    <t>SARA</t>
+  </si>
+  <si>
+    <t>MATHEW</t>
+  </si>
+  <si>
+    <t>HUA ZONG</t>
+  </si>
+  <si>
+    <t>YI HAO</t>
+  </si>
+  <si>
+    <t>MANFRED</t>
+  </si>
+  <si>
+    <t>KIT YIN</t>
+  </si>
+  <si>
+    <t>SUREN</t>
+  </si>
+  <si>
+    <t>HE QUN</t>
+  </si>
+  <si>
+    <t>MALCOLM CHOW</t>
+  </si>
+  <si>
+    <t>BRYAN LEE</t>
+  </si>
+  <si>
+    <t>SEAN YAP</t>
+  </si>
+  <si>
+    <t>KEITH</t>
+  </si>
+  <si>
+    <t>HOWARD</t>
+  </si>
+  <si>
+    <t>CALEB</t>
+  </si>
+  <si>
+    <t>AUGUSTIN</t>
+  </si>
+  <si>
+    <t>MORPHEUS</t>
+  </si>
+  <si>
+    <t>JOSHUR</t>
+  </si>
+  <si>
+    <t>BRENDAN</t>
+  </si>
+  <si>
+    <t>SHIN RON</t>
   </si>
   <si>
     <t>BRAYDEN</t>
@@ -128,271 +211,202 @@
     <t>NOAH LAM</t>
   </si>
   <si>
+    <t>YI LONG</t>
+  </si>
+  <si>
+    <t>MENG LONG</t>
+  </si>
+  <si>
+    <t>KAI</t>
+  </si>
+  <si>
+    <t>CHARLES</t>
+  </si>
+  <si>
+    <t>DARSHAN</t>
+  </si>
+  <si>
+    <t>ZHONG PING</t>
+  </si>
+  <si>
+    <t>DERRILL</t>
+  </si>
+  <si>
+    <t>(SUP) SARAVANAN</t>
+  </si>
+  <si>
+    <t>(SUP) MATHEW YONG</t>
+  </si>
+  <si>
+    <t>(SUP) HUA ZONG</t>
+  </si>
+  <si>
+    <t>(SUP) YI HAO</t>
+  </si>
+  <si>
+    <t>(SUP) MANFRED ONG</t>
+  </si>
+  <si>
+    <t>(CRANE) KIT YIN</t>
+  </si>
+  <si>
+    <t>(RIGG) SURENDREN</t>
+  </si>
+  <si>
+    <t>(CRANE) HE QUN</t>
+  </si>
+  <si>
+    <t>(RIGG) MALCOLM CHOW</t>
+  </si>
+  <si>
+    <t>(RIGG) BRYAN LEE</t>
+  </si>
+  <si>
+    <t>KEITH SHEN</t>
+  </si>
+  <si>
+    <t>HOWARD TAN</t>
+  </si>
+  <si>
+    <t>CALEB TAY</t>
+  </si>
+  <si>
+    <t>BRENDAN HOW</t>
+  </si>
+  <si>
+    <t>REGULAR</t>
+  </si>
+  <si>
+    <t>NSF</t>
+  </si>
+  <si>
+    <t>MAJ</t>
+  </si>
+  <si>
+    <t>JENEVIEVE</t>
+  </si>
+  <si>
+    <t>NAVEEN</t>
+  </si>
+  <si>
+    <t>ROY</t>
+  </si>
+  <si>
+    <t>ELLESTER</t>
+  </si>
+  <si>
+    <t>DANIEL</t>
+  </si>
+  <si>
+    <t>THEOPHILUS</t>
+  </si>
+  <si>
+    <t>JUN YI</t>
+  </si>
+  <si>
+    <t>JAMES</t>
+  </si>
+  <si>
+    <t>ISAAC</t>
+  </si>
+  <si>
+    <t>DEVARAJ</t>
+  </si>
+  <si>
+    <t>PRAVEAN</t>
+  </si>
+  <si>
+    <t>LEONARD</t>
+  </si>
+  <si>
+    <t>IVAN CHEN</t>
+  </si>
+  <si>
+    <t>BRYAN YON</t>
+  </si>
+  <si>
+    <t>JIAN HONG</t>
+  </si>
+  <si>
+    <t>QI XIAN</t>
+  </si>
+  <si>
+    <t>BRYAN CHUA</t>
+  </si>
+  <si>
+    <t>NICHOLAS</t>
+  </si>
+  <si>
+    <t>NISHAN</t>
+  </si>
+  <si>
+    <t>EVAN</t>
+  </si>
+  <si>
+    <t>SEAN TZE</t>
+  </si>
+  <si>
+    <t>ERNEST</t>
+  </si>
+  <si>
+    <t>HERTZ</t>
+  </si>
+  <si>
+    <t>XI QUAN</t>
+  </si>
+  <si>
+    <t>JING XIANG</t>
+  </si>
+  <si>
+    <t>ZACHARY</t>
+  </si>
+  <si>
+    <t>MALCOLM PECK</t>
+  </si>
+  <si>
+    <t>(SUP) DEVARAJ</t>
+  </si>
+  <si>
+    <t>(SUP) PRAVEAN</t>
+  </si>
+  <si>
+    <t>(SUP) LEONARD LOW</t>
+  </si>
+  <si>
+    <t>(SUP) IVAN CHEN</t>
+  </si>
+  <si>
+    <t>(CRANE) BRYAN YON</t>
+  </si>
+  <si>
+    <t>(SUP) JIAN HONG</t>
+  </si>
+  <si>
+    <t>(CRANE) QI XIAN</t>
+  </si>
+  <si>
+    <t>(CRANE) BRYAN CHUA</t>
+  </si>
+  <si>
+    <t>(RIGG) NICHOLAS</t>
+  </si>
+  <si>
+    <t>(RIGG) NISHAN</t>
+  </si>
+  <si>
+    <t>AIK WEE HERTZ</t>
+  </si>
+  <si>
+    <t>ISAAC LIM</t>
+  </si>
+  <si>
+    <t>JIAYING</t>
+  </si>
+  <si>
+    <t>1WO</t>
+  </si>
+  <si>
     <t>MARCUS</t>
-  </si>
-  <si>
-    <t>MENG LONG</t>
-  </si>
-  <si>
-    <t>KAI</t>
-  </si>
-  <si>
-    <t>CHARLES</t>
-  </si>
-  <si>
-    <t>DARSHAN</t>
-  </si>
-  <si>
-    <t>ZHONG PING</t>
-  </si>
-  <si>
-    <t>DERRILL</t>
-  </si>
-  <si>
-    <t>WEI JIAN</t>
-  </si>
-  <si>
-    <t>BRENDON</t>
-  </si>
-  <si>
-    <t>JOVAN</t>
-  </si>
-  <si>
-    <t>RICHMOND</t>
-  </si>
-  <si>
-    <t>MAX</t>
-  </si>
-  <si>
-    <t>LEON</t>
-  </si>
-  <si>
-    <t>YEN KIT</t>
-  </si>
-  <si>
-    <t>AIDAN</t>
-  </si>
-  <si>
-    <t>GUAN LIN</t>
-  </si>
-  <si>
-    <t>SARA</t>
-  </si>
-  <si>
-    <t>MATHEW</t>
-  </si>
-  <si>
-    <t>HUA ZONG</t>
-  </si>
-  <si>
-    <t>YI HAO</t>
-  </si>
-  <si>
-    <t>MANFRED</t>
-  </si>
-  <si>
-    <t>KIT YIN</t>
-  </si>
-  <si>
-    <t>SUREN</t>
-  </si>
-  <si>
-    <t>HE QUN</t>
-  </si>
-  <si>
-    <t>MALCOLM CHOW</t>
-  </si>
-  <si>
-    <t>BRYAN LEE</t>
-  </si>
-  <si>
-    <t>SEAN YAP</t>
-  </si>
-  <si>
-    <t>KEITH</t>
-  </si>
-  <si>
-    <t>HOWARD</t>
-  </si>
-  <si>
-    <t>CALEB</t>
-  </si>
-  <si>
-    <t>AUGUSTIN</t>
-  </si>
-  <si>
-    <t>MORPHEUS</t>
-  </si>
-  <si>
-    <t>JOSHUR</t>
-  </si>
-  <si>
-    <t>BRENDAN</t>
-  </si>
-  <si>
-    <t>SHIN RON</t>
-  </si>
-  <si>
-    <t>(SUP) SARAVANAN</t>
-  </si>
-  <si>
-    <t>(SUP) MATHEW YONG</t>
-  </si>
-  <si>
-    <t>(SUP) HUA ZONG</t>
-  </si>
-  <si>
-    <t>(SUP) YI HAO</t>
-  </si>
-  <si>
-    <t>(SUP) MANFRED ONG</t>
-  </si>
-  <si>
-    <t>(CRANE) KIT YIN</t>
-  </si>
-  <si>
-    <t>(RIGG) SURENDREN</t>
-  </si>
-  <si>
-    <t>(CRANE) HE QUN</t>
-  </si>
-  <si>
-    <t>(RIGG) MALCOLM CHOW</t>
-  </si>
-  <si>
-    <t>(RIGG) BRYAN LEE</t>
-  </si>
-  <si>
-    <t>KEITH SHEN</t>
-  </si>
-  <si>
-    <t>HOWARD TAN</t>
-  </si>
-  <si>
-    <t>CALEB TAY</t>
-  </si>
-  <si>
-    <t>BRENDAN HOW</t>
-  </si>
-  <si>
-    <t>REGULAR</t>
-  </si>
-  <si>
-    <t>NSF</t>
-  </si>
-  <si>
-    <t>MAJ</t>
-  </si>
-  <si>
-    <t>JENEVIEVE</t>
-  </si>
-  <si>
-    <t>NAVEEN</t>
-  </si>
-  <si>
-    <t>ROY</t>
-  </si>
-  <si>
-    <t>DANIEL</t>
-  </si>
-  <si>
-    <t>THEOPHILUS</t>
-  </si>
-  <si>
-    <t>DEVARAJ</t>
-  </si>
-  <si>
-    <t>PRAVEAN</t>
-  </si>
-  <si>
-    <t>LEONARD</t>
-  </si>
-  <si>
-    <t>IVAN CHEN</t>
-  </si>
-  <si>
-    <t>BRYAN YON</t>
-  </si>
-  <si>
-    <t>JIAN HONG</t>
-  </si>
-  <si>
-    <t>QI XIAN</t>
-  </si>
-  <si>
-    <t>BRYAN CHUA</t>
-  </si>
-  <si>
-    <t>NICHOLAS</t>
-  </si>
-  <si>
-    <t>NISHAN</t>
-  </si>
-  <si>
-    <t>EVAN</t>
-  </si>
-  <si>
-    <t>SEAN TZE</t>
-  </si>
-  <si>
-    <t>ERNEST</t>
-  </si>
-  <si>
-    <t>HERTZ</t>
-  </si>
-  <si>
-    <t>XI QUAN</t>
-  </si>
-  <si>
-    <t>JING XIANG</t>
-  </si>
-  <si>
-    <t>ISAAC</t>
-  </si>
-  <si>
-    <t>ZACHARY</t>
-  </si>
-  <si>
-    <t>MALCOLM PECK</t>
-  </si>
-  <si>
-    <t>(SUP) DEVARAJ</t>
-  </si>
-  <si>
-    <t>(SUP) PRAVEAN</t>
-  </si>
-  <si>
-    <t>(SUP) LEONARD LOW</t>
-  </si>
-  <si>
-    <t>(SUP) IVAN CHEN</t>
-  </si>
-  <si>
-    <t>(CRANE) BRYAN YON</t>
-  </si>
-  <si>
-    <t>(SUP) JIAN HONG</t>
-  </si>
-  <si>
-    <t>(CRANE) QI XIAN</t>
-  </si>
-  <si>
-    <t>(CRANE) BRYAN CHUA</t>
-  </si>
-  <si>
-    <t>(RIGG) NICHOLAS</t>
-  </si>
-  <si>
-    <t>(RIGG) NISHAN</t>
-  </si>
-  <si>
-    <t>AIK WEE HERTZ</t>
-  </si>
-  <si>
-    <t>JIAYING</t>
-  </si>
-  <si>
-    <t>1WO</t>
   </si>
   <si>
     <t>KENNETH</t>
@@ -565,49 +579,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="personnel_edit_instructions.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="7562850" cy="10696575"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -895,22 +866,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -995,7 +953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E41"/>
   <sheetViews>
@@ -1049,13 +1007,13 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>85</v>
@@ -1066,16 +1024,16 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1083,27 +1041,27 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -1114,13 +1072,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -1131,13 +1089,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -1148,30 +1106,30 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -1182,13 +1140,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -1199,47 +1157,47 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
         <v>43</v>
@@ -1250,47 +1208,47 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
         <v>45</v>
       </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
@@ -1301,101 +1259,101 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
         <v>85</v>
@@ -1403,160 +1361,160 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
         <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
         <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D32" t="s">
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>62</v>
@@ -1568,18 +1526,18 @@
         <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D34" t="s">
         <v>22</v>
@@ -1590,13 +1548,13 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
         <v>22</v>
@@ -1613,7 +1571,7 @@
         <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D36" t="s">
         <v>22</v>
@@ -1681,7 +1639,7 @@
         <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
         <v>22</v>
@@ -1712,9 +1670,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1763,7 +1721,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -1772,7 +1730,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
         <v>85</v>
@@ -1780,7 +1738,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -1797,7 +1755,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>88</v>
@@ -1814,7 +1772,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>89</v>
@@ -1831,7 +1789,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>90</v>
@@ -1848,7 +1806,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>91</v>
@@ -1860,12 +1818,12 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>92</v>
@@ -1882,13 +1840,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -1899,84 +1857,84 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="E15" t="s">
         <v>85</v>
@@ -1984,16 +1942,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="E16" t="s">
         <v>85</v>
@@ -2001,16 +1959,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>99</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="E17" t="s">
         <v>85</v>
@@ -2018,13 +1976,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
@@ -2035,13 +1993,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -2052,13 +2010,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -2069,75 +2027,75 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
         <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>107</v>
@@ -2154,7 +2112,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>108</v>
@@ -2171,7 +2129,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>109</v>
@@ -2188,13 +2146,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
         <v>110</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
@@ -2205,7 +2163,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>111</v>
@@ -2217,6 +2175,74 @@
         <v>22</v>
       </c>
       <c r="E29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2225,7 +2251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -2259,16 +2285,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="E2" t="s">
         <v>85</v>
@@ -2276,7 +2302,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -2285,7 +2311,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="E3" t="s">
         <v>85</v>
@@ -2293,16 +2319,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E4" t="s">
         <v>85</v>
@@ -2310,16 +2336,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="E5" t="s">
         <v>85</v>
@@ -2327,16 +2353,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D6" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E6" t="s">
         <v>85</v>
@@ -2344,16 +2370,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
         <v>85</v>
@@ -2361,16 +2387,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D8" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E8" t="s">
         <v>85</v>
@@ -2378,16 +2404,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="E9" t="s">
         <v>85</v>
@@ -2395,16 +2421,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E10" t="s">
         <v>85</v>
@@ -2412,16 +2438,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E11" t="s">
         <v>85</v>
@@ -2429,16 +2455,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E12" t="s">
         <v>85</v>
@@ -2446,16 +2472,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C13" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E13" t="s">
         <v>85</v>
@@ -2463,16 +2489,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D14" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E14" t="s">
         <v>85</v>
@@ -2480,16 +2506,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E15" t="s">
         <v>85</v>
@@ -2497,16 +2523,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="E16" t="s">
         <v>85</v>
@@ -2514,13 +2540,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
@@ -2531,13 +2557,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
@@ -2548,13 +2574,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -2565,13 +2591,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C20" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -2582,13 +2608,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -2599,13 +2625,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -2616,13 +2642,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>

</xml_diff>